<commit_message>
Initial draft of blog 2 and supporting images and code updates.
</commit_message>
<xml_diff>
--- a/EquiRectangular/src/DPC++/Flatten360Image-Results.xlsx
+++ b/EquiRectangular/src/DPC++/Flatten360Image-Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dpbogia\source\repos\flatten360image\EquiRectangular\src\DPC++\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB2770A-46D2-4E53-BEBC-B87ACEE4D3CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7DD73552-016C-44FA-A9E9-041400E6BAEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12" yWindow="12" windowWidth="23016" windowHeight="12936" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Python" sheetId="4" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Config" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -864,6 +865,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -873,7 +875,6 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -919,28 +920,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -1274,7 +1254,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2765D98F-BCB6-4667-8355-EC9FF295E740}">
   <dimension ref="A1:P85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1292,14 +1272,14 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="G3" s="9" t="s">
+      <c r="C3" s="9"/>
+      <c r="G3" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="9"/>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -2375,8 +2355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E039E1D5-1AC2-402C-B7E5-C5A4311AD27A}">
   <dimension ref="A1:BA281"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I237" workbookViewId="0">
-      <selection activeCell="U250" sqref="U250:V250"/>
+    <sheetView topLeftCell="I231" workbookViewId="0">
+      <selection activeCell="X251" sqref="X251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2392,62 +2372,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" s="5" customFormat="1" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="N1" s="10" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="N1" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="AA1" s="10" t="s">
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="AA1" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="AB1" s="10"/>
-      <c r="AC1" s="10"/>
-      <c r="AD1" s="10"/>
-      <c r="AE1" s="10"/>
-      <c r="AF1" s="10"/>
-      <c r="AG1" s="10"/>
-      <c r="AH1" s="10"/>
-      <c r="AI1" s="10"/>
-      <c r="AJ1" s="10"/>
-      <c r="AK1" s="10"/>
+      <c r="AB1" s="11"/>
+      <c r="AC1" s="11"/>
+      <c r="AD1" s="11"/>
+      <c r="AE1" s="11"/>
+      <c r="AF1" s="11"/>
+      <c r="AG1" s="11"/>
+      <c r="AH1" s="11"/>
+      <c r="AI1" s="11"/>
+      <c r="AJ1" s="11"/>
+      <c r="AK1" s="11"/>
       <c r="AL1" s="6"/>
       <c r="AM1" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="AO1" s="10" t="s">
+      <c r="AO1" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="AP1" s="10"/>
-      <c r="AQ1" s="10"/>
-      <c r="AR1" s="10"/>
-      <c r="AS1" s="10"/>
-      <c r="AT1" s="10"/>
-      <c r="AU1" s="10"/>
-      <c r="AV1" s="10"/>
-      <c r="AW1" s="10"/>
-      <c r="AX1" s="10"/>
-      <c r="AY1" s="10"/>
+      <c r="AP1" s="11"/>
+      <c r="AQ1" s="11"/>
+      <c r="AR1" s="11"/>
+      <c r="AS1" s="11"/>
+      <c r="AT1" s="11"/>
+      <c r="AU1" s="11"/>
+      <c r="AV1" s="11"/>
+      <c r="AW1" s="11"/>
+      <c r="AX1" s="11"/>
+      <c r="AY1" s="11"/>
       <c r="AZ1" s="6"/>
       <c r="BA1" s="5" t="s">
         <v>58</v>
@@ -2567,7 +2547,7 @@
       <c r="AK4">
         <v>0.14024987999999999</v>
       </c>
-      <c r="AM4" s="11">
+      <c r="AM4" s="8">
         <f>K4/AK4</f>
         <v>6.427940116597604</v>
       </c>
@@ -2604,7 +2584,7 @@
       <c r="AY4">
         <v>0.13594837000000001</v>
       </c>
-      <c r="BA4" s="11">
+      <c r="BA4" s="8">
         <f>X4/AY4</f>
         <v>6.7720761933372202</v>
       </c>
@@ -2709,7 +2689,7 @@
       <c r="AK5">
         <v>0.14063440999999999</v>
       </c>
-      <c r="AM5" s="11">
+      <c r="AM5" s="8">
         <f>K5/AK5</f>
         <v>6.5759047874556451</v>
       </c>
@@ -2746,7 +2726,7 @@
       <c r="AY5">
         <v>0.13530285</v>
       </c>
-      <c r="BA5" s="11">
+      <c r="BA5" s="8">
         <f>X5/AY5</f>
         <v>6.8045939904443991</v>
       </c>
@@ -2865,7 +2845,7 @@
       <c r="AK8">
         <v>12.98160118</v>
       </c>
-      <c r="AM8" s="11">
+      <c r="AM8" s="8">
         <f>K8/AK8</f>
         <v>2.8286930264483749</v>
       </c>
@@ -2902,7 +2882,7 @@
       <c r="AY8">
         <v>12.97781054</v>
       </c>
-      <c r="BA8" s="11">
+      <c r="BA8" s="8">
         <f>X8/AY8</f>
         <v>2.8579386981866048</v>
       </c>
@@ -3007,7 +2987,7 @@
       <c r="AK9">
         <v>15.03761841</v>
       </c>
-      <c r="AM9" s="11">
+      <c r="AM9" s="8">
         <f>K9/AK9</f>
         <v>4.3041218466455282</v>
       </c>
@@ -3044,7 +3024,7 @@
       <c r="AY9">
         <v>63.851321429999999</v>
       </c>
-      <c r="BA9" s="11">
+      <c r="BA9" s="8">
         <f>X9/AY9</f>
         <v>5.4194899624648221</v>
       </c>
@@ -3163,7 +3143,7 @@
       <c r="AK12">
         <v>14.15113697</v>
       </c>
-      <c r="AM12" s="11">
+      <c r="AM12" s="8">
         <f>K12/AK12</f>
         <v>3.1113268526295665</v>
       </c>
@@ -3200,7 +3180,7 @@
       <c r="AY12">
         <v>13.74914412</v>
       </c>
-      <c r="BA12" s="11">
+      <c r="BA12" s="8">
         <f>X12/AY12</f>
         <v>3.2064312189346662</v>
       </c>
@@ -3305,7 +3285,7 @@
       <c r="AK13">
         <v>14.4571858</v>
       </c>
-      <c r="AM13" s="11">
+      <c r="AM13" s="8">
         <f>K13/AK13</f>
         <v>3.9310800301120845</v>
       </c>
@@ -3342,7 +3322,7 @@
       <c r="AY13">
         <v>51.692949259999999</v>
       </c>
-      <c r="BA13" s="11">
+      <c r="BA13" s="8">
         <f>X13/AY13</f>
         <v>3.7867461714255461</v>
       </c>
@@ -3461,7 +3441,7 @@
       <c r="AK16">
         <v>14.99623594</v>
       </c>
-      <c r="AM16" s="11">
+      <c r="AM16" s="8">
         <f>K16/AK16</f>
         <v>3.3576737170220863</v>
       </c>
@@ -3498,7 +3478,7 @@
       <c r="AY16">
         <v>14.650876930000001</v>
       </c>
-      <c r="BA16" s="11">
+      <c r="BA16" s="8">
         <f>X16/AY16</f>
         <v>3.3909779658493107</v>
       </c>
@@ -3603,7 +3583,7 @@
       <c r="AK17">
         <v>15.17639524</v>
       </c>
-      <c r="AM17" s="11">
+      <c r="AM17" s="8">
         <f>K17/AK17</f>
         <v>4.2399361220115406</v>
       </c>
@@ -3640,7 +3620,7 @@
       <c r="AY17">
         <v>64.314459630000002</v>
       </c>
-      <c r="BA17" s="11">
+      <c r="BA17" s="8">
         <f>X17/AY17</f>
         <v>5.4249582365650673</v>
       </c>
@@ -3759,7 +3739,7 @@
       <c r="AK20">
         <v>14.26934531</v>
       </c>
-      <c r="AM20" s="11">
+      <c r="AM20" s="8">
         <f>K20/AK20</f>
         <v>3.1007610278372328</v>
       </c>
@@ -3796,7 +3776,7 @@
       <c r="AY20">
         <v>13.94783788</v>
       </c>
-      <c r="BA20" s="11">
+      <c r="BA20" s="8">
         <f>X20/AY20</f>
         <v>3.1876656161707553</v>
       </c>
@@ -3901,7 +3881,7 @@
       <c r="AK21">
         <v>14.49345561</v>
       </c>
-      <c r="AM21" s="11">
+      <c r="AM21" s="8">
         <f>K21/AK21</f>
         <v>3.9150212003857652</v>
       </c>
@@ -3938,7 +3918,7 @@
       <c r="AY21">
         <v>51.802955230000002</v>
       </c>
-      <c r="BA21" s="11">
+      <c r="BA21" s="8">
         <f>X21/AY21</f>
         <v>3.7681224546617433</v>
       </c>
@@ -4057,7 +4037,7 @@
       <c r="AK24">
         <v>27.95732594</v>
       </c>
-      <c r="AM24" s="11">
+      <c r="AM24" s="8">
         <f>K24/AK24</f>
         <v>3.1976113209774306</v>
       </c>
@@ -4094,7 +4074,7 @@
       <c r="AY24">
         <v>27.883969230000002</v>
       </c>
-      <c r="BA24" s="11">
+      <c r="BA24" s="8">
         <f>X24/AY24</f>
         <v>3.1282514257745073</v>
       </c>
@@ -4199,7 +4179,7 @@
       <c r="AK25">
         <v>28.924303420000001</v>
       </c>
-      <c r="AM25" s="11">
+      <c r="AM25" s="8">
         <f>K25/AK25</f>
         <v>4.7864466580125509</v>
       </c>
@@ -4236,7 +4216,7 @@
       <c r="AY25">
         <v>64.118367640000002</v>
       </c>
-      <c r="BA25" s="11">
+      <c r="BA25" s="8">
         <f>X25/AY25</f>
         <v>5.4265124736728243</v>
       </c>
@@ -4355,7 +4335,7 @@
       <c r="AK28">
         <v>25.478940380000001</v>
       </c>
-      <c r="AM28" s="11">
+      <c r="AM28" s="8">
         <f>K28/AK28</f>
         <v>2.7313096307029392</v>
       </c>
@@ -4392,7 +4372,7 @@
       <c r="AY28">
         <v>25.2957708</v>
       </c>
-      <c r="BA28" s="11">
+      <c r="BA28" s="8">
         <f>X28/AY28</f>
         <v>2.8366831466546971</v>
       </c>
@@ -4497,7 +4477,7 @@
       <c r="AK29">
         <v>26.33713711</v>
       </c>
-      <c r="AM29" s="11">
+      <c r="AM29" s="8">
         <f>K29/AK29</f>
         <v>4.0384657886606563</v>
       </c>
@@ -4534,7 +4514,7 @@
       <c r="AY29">
         <v>51.61441902</v>
       </c>
-      <c r="BA29" s="11">
+      <c r="BA29" s="8">
         <f>X29/AY29</f>
         <v>3.7849083316098517</v>
       </c>
@@ -4653,7 +4633,7 @@
       <c r="AK32">
         <v>24.709844650000001</v>
       </c>
-      <c r="AM32" s="11">
+      <c r="AM32" s="8">
         <f>K32/AK32</f>
         <v>5.4752414965101774</v>
       </c>
@@ -4690,7 +4670,7 @@
       <c r="AY32">
         <v>24.81962339</v>
       </c>
-      <c r="BA32" s="11">
+      <c r="BA32" s="8">
         <f>X32/AY32</f>
         <v>5.3938846265467042</v>
       </c>
@@ -4795,7 +4775,7 @@
       <c r="AK33">
         <v>25.49802292</v>
       </c>
-      <c r="AM33" s="11">
+      <c r="AM33" s="8">
         <f>K33/AK33</f>
         <v>6.5142149703581804</v>
       </c>
@@ -4832,7 +4812,7 @@
       <c r="AY33">
         <v>65.63734187</v>
       </c>
-      <c r="BA33" s="11">
+      <c r="BA33" s="8">
         <f>X33/AY33</f>
         <v>5.3834202347780113</v>
       </c>
@@ -4951,7 +4931,7 @@
       <c r="AK36">
         <v>25.407859670000001</v>
       </c>
-      <c r="AM36" s="11">
+      <c r="AM36" s="8">
         <f>K36/AK36</f>
         <v>5.3692072623132532</v>
       </c>
@@ -4988,7 +4968,7 @@
       <c r="AY36">
         <v>25.23856756</v>
       </c>
-      <c r="BA36" s="11">
+      <c r="BA36" s="8">
         <f>X36/AY36</f>
         <v>5.2651588638733351</v>
       </c>
@@ -5093,7 +5073,7 @@
       <c r="AK37">
         <v>25.94033924</v>
       </c>
-      <c r="AM37" s="11">
+      <c r="AM37" s="8">
         <f>K37/AK37</f>
         <v>6.451596206264572</v>
       </c>
@@ -5130,7 +5110,7 @@
       <c r="AY37">
         <v>68.958854389999999</v>
       </c>
-      <c r="BA37" s="11">
+      <c r="BA37" s="8">
         <f>X37/AY37</f>
         <v>5.2733134299680762</v>
       </c>
@@ -5249,7 +5229,7 @@
       <c r="AK40">
         <v>1.8959153799999999</v>
       </c>
-      <c r="AM40" s="11">
+      <c r="AM40" s="8">
         <f>K40/AK40</f>
         <v>0.60716905519274811</v>
       </c>
@@ -5286,7 +5266,7 @@
       <c r="AY40">
         <v>2.0028825499999998</v>
       </c>
-      <c r="BA40" s="11">
+      <c r="BA40" s="8">
         <f>X40/AY40</f>
         <v>1.4697526123037021</v>
       </c>
@@ -5391,7 +5371,7 @@
       <c r="AK41">
         <v>5.1724745299999997</v>
       </c>
-      <c r="AM41" s="11">
+      <c r="AM41" s="8">
         <f>K41/AK41</f>
         <v>42.565558293817261</v>
       </c>
@@ -5428,7 +5408,7 @@
       <c r="AY41">
         <v>65.866463780000004</v>
       </c>
-      <c r="BA41" s="11">
+      <c r="BA41" s="8">
         <f>X41/AY41</f>
         <v>5.4540661303739419</v>
       </c>
@@ -5547,7 +5527,7 @@
       <c r="AK44">
         <v>3.3409652099999998</v>
       </c>
-      <c r="AM44" s="11">
+      <c r="AM44" s="8">
         <f>K44/AK44</f>
         <v>1.0819799018499807</v>
       </c>
@@ -5584,7 +5564,7 @@
       <c r="AY44">
         <v>2.4789020599999998</v>
       </c>
-      <c r="BA44" s="11">
+      <c r="BA44" s="8">
         <f>X44/AY44</f>
         <v>2.2004996639520322</v>
       </c>
@@ -5689,7 +5669,7 @@
       <c r="AK45">
         <v>20.206519929999999</v>
       </c>
-      <c r="AM45" s="11">
+      <c r="AM45" s="8">
         <f>K45/AK45</f>
         <v>10.667183043725631</v>
       </c>
@@ -5726,7 +5706,7 @@
       <c r="AY45">
         <v>66.269649610000002</v>
       </c>
-      <c r="BA45" s="11">
+      <c r="BA45" s="8">
         <f>X45/AY45</f>
         <v>5.4288073319722505</v>
       </c>
@@ -5845,7 +5825,7 @@
       <c r="AK48">
         <v>2.5476843699999998</v>
       </c>
-      <c r="AM48" s="11">
+      <c r="AM48" s="8">
         <f>K48/AK48</f>
         <v>1.9051722368575825</v>
       </c>
@@ -5882,7 +5862,7 @@
       <c r="AY48">
         <v>2.57732224</v>
       </c>
-      <c r="BA48" s="11">
+      <c r="BA48" s="8">
         <f>X48/AY48</f>
         <v>1.8685421501659025</v>
       </c>
@@ -5987,7 +5967,7 @@
       <c r="AK49">
         <v>5.5139965000000002</v>
       </c>
-      <c r="AM49" s="11">
+      <c r="AM49" s="8">
         <f>K49/AK49</f>
         <v>39.544001924919613</v>
       </c>
@@ -6024,7 +6004,7 @@
       <c r="AY49">
         <v>66.17633094</v>
       </c>
-      <c r="BA49" s="11">
+      <c r="BA49" s="8">
         <f>X49/AY49</f>
         <v>5.4175201032987337</v>
       </c>
@@ -6143,7 +6123,7 @@
       <c r="AK52">
         <v>3.3715146100000002</v>
       </c>
-      <c r="AM52" s="11">
+      <c r="AM52" s="8">
         <f>K52/AK52</f>
         <v>1.5910662893434711</v>
       </c>
@@ -6180,7 +6160,7 @@
       <c r="AY52">
         <v>2.78156998</v>
       </c>
-      <c r="BA52" s="11">
+      <c r="BA52" s="8">
         <f>X52/AY52</f>
         <v>1.9272137636458098</v>
       </c>
@@ -6285,7 +6265,7 @@
       <c r="AK53">
         <v>20.20934252</v>
       </c>
-      <c r="AM53" s="11">
+      <c r="AM53" s="8">
         <f>K53/AK53</f>
         <v>10.692996312776632</v>
       </c>
@@ -6322,7 +6302,7 @@
       <c r="AY53">
         <v>66.072468150000006</v>
       </c>
-      <c r="BA53" s="11">
+      <c r="BA53" s="8">
         <f>X53/AY53</f>
         <v>5.4669860069394112</v>
       </c>
@@ -6441,7 +6421,7 @@
       <c r="AK56">
         <v>4.5396087700000001</v>
       </c>
-      <c r="AM56" s="11">
+      <c r="AM56" s="8">
         <f>K56/AK56</f>
         <v>1.334960494844581</v>
       </c>
@@ -6478,7 +6458,7 @@
       <c r="AY56">
         <v>4.2746533099999997</v>
       </c>
-      <c r="BA56" s="11">
+      <c r="BA56" s="8">
         <f>X56/AY56</f>
         <v>1.4259449148169634</v>
       </c>
@@ -6583,7 +6563,7 @@
       <c r="AK57">
         <v>9.8523999199999999</v>
       </c>
-      <c r="AM57" s="11">
+      <c r="AM57" s="8">
         <f>K57/AK57</f>
         <v>31.300532938577668</v>
       </c>
@@ -6620,7 +6600,7 @@
       <c r="AY57">
         <v>66.215320969999993</v>
       </c>
-      <c r="BA57" s="11">
+      <c r="BA57" s="8">
         <f>X57/AY57</f>
         <v>5.4100203756816443</v>
       </c>
@@ -6739,7 +6719,7 @@
       <c r="AK60">
         <v>9.2952957400000003</v>
       </c>
-      <c r="AM60" s="11">
+      <c r="AM60" s="8">
         <f>K60/AK60</f>
         <v>12.603540388269561</v>
       </c>
@@ -6776,7 +6756,7 @@
       <c r="AY60">
         <v>9.4601919900000002</v>
       </c>
-      <c r="BA60" s="11">
+      <c r="BA60" s="8">
         <f>X60/AY60</f>
         <v>14.373568838109806</v>
       </c>
@@ -6881,7 +6861,7 @@
       <c r="AK61">
         <v>9.6740894999999991</v>
       </c>
-      <c r="AM61" s="11">
+      <c r="AM61" s="8">
         <f>K61/AK61</f>
         <v>28.812426246418337</v>
       </c>
@@ -6918,7 +6898,7 @@
       <c r="AY61">
         <v>65.862928179999997</v>
       </c>
-      <c r="BA61" s="11">
+      <c r="BA61" s="8">
         <f>X61/AY61</f>
         <v>5.4211889517603291</v>
       </c>
@@ -7037,7 +7017,7 @@
       <c r="AK64">
         <v>4.72414311</v>
       </c>
-      <c r="AM64" s="11">
+      <c r="AM64" s="8">
         <f>K64/AK64</f>
         <v>1.8626694566837538</v>
       </c>
@@ -7074,7 +7054,7 @@
       <c r="AY64">
         <v>4.7279624900000004</v>
       </c>
-      <c r="BA64" s="11">
+      <c r="BA64" s="8">
         <f>X64/AY64</f>
         <v>1.8771192281603741</v>
       </c>
@@ -7179,7 +7159,7 @@
       <c r="AK65">
         <v>27.2798999</v>
       </c>
-      <c r="AM65" s="11">
+      <c r="AM65" s="8">
         <f>K65/AK65</f>
         <v>10.938484089525563</v>
       </c>
@@ -7216,7 +7196,7 @@
       <c r="AY65">
         <v>66.149212250000005</v>
       </c>
-      <c r="BA65" s="11">
+      <c r="BA65" s="8">
         <f>X65/AY65</f>
         <v>5.4480564995692742</v>
       </c>
@@ -7335,7 +7315,7 @@
       <c r="AK68">
         <v>24.951095850000002</v>
       </c>
-      <c r="AM68" s="11">
+      <c r="AM68" s="8">
         <f>K68/AK68</f>
         <v>7.1566015506288876</v>
       </c>
@@ -7372,7 +7352,7 @@
       <c r="AY68">
         <v>24.21330957</v>
       </c>
-      <c r="BA68" s="11">
+      <c r="BA68" s="8">
         <f>X68/AY68</f>
         <v>7.5091547123849045</v>
       </c>
@@ -7477,7 +7457,7 @@
       <c r="AK69">
         <v>26.73434091</v>
       </c>
-      <c r="AM69" s="11">
+      <c r="AM69" s="8">
         <f>K69/AK69</f>
         <v>9.4651867544394221</v>
       </c>
@@ -7514,7 +7494,7 @@
       <c r="AY69">
         <v>66.410186100000004</v>
       </c>
-      <c r="BA69" s="11">
+      <c r="BA69" s="8">
         <f>X69/AY69</f>
         <v>5.4224417665048517</v>
       </c>
@@ -7633,7 +7613,7 @@
       <c r="AK72">
         <v>4.4683451300000003</v>
       </c>
-      <c r="AM72" s="11">
+      <c r="AM72" s="8">
         <f>K72/AK72</f>
         <v>1.3545134191548001</v>
       </c>
@@ -7670,7 +7650,7 @@
       <c r="AY72">
         <v>4.45943807</v>
       </c>
-      <c r="BA72" s="11">
+      <c r="BA72" s="8">
         <f>X72/AY72</f>
         <v>1.3805725482358813</v>
       </c>
@@ -7775,7 +7755,7 @@
       <c r="AK73">
         <v>9.6384684699999994</v>
       </c>
-      <c r="AM73" s="11">
+      <c r="AM73" s="8">
         <f>K73/AK73</f>
         <v>31.986349424661238</v>
       </c>
@@ -7812,7 +7792,7 @@
       <c r="AY73">
         <v>66.281504839999997</v>
       </c>
-      <c r="BA73" s="11">
+      <c r="BA73" s="8">
         <f>X73/AY73</f>
         <v>5.4109741836090759</v>
       </c>
@@ -7931,7 +7911,7 @@
       <c r="AK76">
         <v>9.2614459900000004</v>
       </c>
-      <c r="AM76" s="11">
+      <c r="AM76" s="8">
         <f>K76/AK76</f>
         <v>15.05143788999195</v>
       </c>
@@ -7968,7 +7948,7 @@
       <c r="AY76">
         <v>9.5088851000000005</v>
       </c>
-      <c r="BA76" s="11">
+      <c r="BA76" s="8">
         <f>X76/AY76</f>
         <v>14.704867377143929</v>
       </c>
@@ -8073,7 +8053,7 @@
       <c r="AK77">
         <v>9.4703329000000007</v>
       </c>
-      <c r="AM77" s="11">
+      <c r="AM77" s="8">
         <f>K77/AK77</f>
         <v>29.481267664835727</v>
       </c>
@@ -8110,7 +8090,7 @@
       <c r="AY77">
         <v>66.136520730000001</v>
       </c>
-      <c r="BA77" s="11">
+      <c r="BA77" s="8">
         <f>X77/AY77</f>
         <v>5.4373017454013262</v>
       </c>
@@ -8229,7 +8209,7 @@
       <c r="AK80">
         <v>4.6345216200000001</v>
       </c>
-      <c r="AM80" s="11">
+      <c r="AM80" s="8">
         <f>K80/AK80</f>
         <v>1.8517593580672518</v>
       </c>
@@ -8266,7 +8246,7 @@
       <c r="AY80">
         <v>4.61634908</v>
       </c>
-      <c r="BA80" s="11">
+      <c r="BA80" s="8">
         <f>X80/AY80</f>
         <v>1.8629131140143329</v>
       </c>
@@ -8371,7 +8351,7 @@
       <c r="AK81">
         <v>27.300585529999999</v>
       </c>
-      <c r="AM81" s="11">
+      <c r="AM81" s="8">
         <f>K81/AK81</f>
         <v>10.868136809884751</v>
       </c>
@@ -8408,7 +8388,7 @@
       <c r="AY81">
         <v>66.269522260000002</v>
       </c>
-      <c r="BA81" s="11">
+      <c r="BA81" s="8">
         <f>X81/AY81</f>
         <v>5.4412208754920934</v>
       </c>
@@ -8527,7 +8507,7 @@
       <c r="AK84">
         <v>24.808909379999999</v>
       </c>
-      <c r="AM84" s="11">
+      <c r="AM84" s="8">
         <f>K84/AK84</f>
         <v>7.4553508659718437</v>
       </c>
@@ -8564,7 +8544,7 @@
       <c r="AY84">
         <v>25.504153349999999</v>
       </c>
-      <c r="BA84" s="11">
+      <c r="BA84" s="8">
         <f>X84/AY84</f>
         <v>7.6568700207411515</v>
       </c>
@@ -8669,7 +8649,7 @@
       <c r="AK85">
         <v>26.6292437</v>
       </c>
-      <c r="AM85" s="11">
+      <c r="AM85" s="8">
         <f>K85/AK85</f>
         <v>9.4045553854764563</v>
       </c>
@@ -8706,7 +8686,7 @@
       <c r="AY85">
         <v>66.266360419999998</v>
       </c>
-      <c r="BA85" s="11">
+      <c r="BA85" s="8">
         <f>X85/AY85</f>
         <v>5.4258364310511205</v>
       </c>
@@ -8825,7 +8805,7 @@
       <c r="AK88">
         <v>2.3257074200000001</v>
       </c>
-      <c r="AM88" s="11">
+      <c r="AM88" s="8">
         <f>K88/AK88</f>
         <v>1.7000602939126366</v>
       </c>
@@ -8862,7 +8842,7 @@
       <c r="AY88">
         <v>2.3325443099999998</v>
       </c>
-      <c r="BA88" s="11">
+      <c r="BA88" s="8">
         <f>X88/AY88</f>
         <v>1.6880884676527326</v>
       </c>
@@ -8967,7 +8947,7 @@
       <c r="AK89">
         <v>3.8195613000000002</v>
       </c>
-      <c r="AM89" s="11">
+      <c r="AM89" s="8">
         <f>K89/AK89</f>
         <v>52.127004116938764</v>
       </c>
@@ -9004,7 +8984,7 @@
       <c r="AY89">
         <v>66.374512609999996</v>
       </c>
-      <c r="BA89" s="11">
+      <c r="BA89" s="8">
         <f>X89/AY89</f>
         <v>5.3912415546097376</v>
       </c>
@@ -9123,7 +9103,7 @@
       <c r="AK92">
         <v>3.7381794099999999</v>
       </c>
-      <c r="AM92" s="11">
+      <c r="AM92" s="8">
         <f>K92/AK92</f>
         <v>29.450739265079843</v>
       </c>
@@ -9160,7 +9140,7 @@
       <c r="AY92">
         <v>3.9823073999999998</v>
       </c>
-      <c r="BA92" s="11">
+      <c r="BA92" s="8">
         <f>X92/AY92</f>
         <v>27.006377609121788</v>
       </c>
@@ -9265,7 +9245,7 @@
       <c r="AK93">
         <v>3.7434881799999999</v>
       </c>
-      <c r="AM93" s="11">
+      <c r="AM93" s="8">
         <f>K93/AK93</f>
         <v>52.081213799905733</v>
       </c>
@@ -9302,7 +9282,7 @@
       <c r="AY93">
         <v>66.311049350000005</v>
       </c>
-      <c r="BA93" s="11">
+      <c r="BA93" s="8">
         <f>X93/AY93</f>
         <v>5.3764119351852777</v>
       </c>
@@ -9421,7 +9401,7 @@
       <c r="AK96">
         <v>3.3835932299999998</v>
       </c>
-      <c r="AM96" s="11">
+      <c r="AM96" s="8">
         <f>K96/AK96</f>
         <v>2.2097360503348686</v>
       </c>
@@ -9458,7 +9438,7 @@
       <c r="AY96">
         <v>3.3054081399999999</v>
       </c>
-      <c r="BA96" s="11">
+      <c r="BA96" s="8">
         <f>X96/AY96</f>
         <v>2.2837635778315715</v>
       </c>
@@ -9563,7 +9543,7 @@
       <c r="AK97">
         <v>13.351491360000001</v>
       </c>
-      <c r="AM97" s="11">
+      <c r="AM97" s="8">
         <f>K97/AK97</f>
         <v>15.139696233904465</v>
       </c>
@@ -9600,7 +9580,7 @@
       <c r="AY97">
         <v>66.432633359999997</v>
       </c>
-      <c r="BA97" s="11">
+      <c r="BA97" s="8">
         <f>X97/AY97</f>
         <v>5.4059119808463967</v>
       </c>
@@ -9719,7 +9699,7 @@
       <c r="AK100">
         <v>12.735884499999999</v>
       </c>
-      <c r="AM100" s="11">
+      <c r="AM100" s="8">
         <f>K100/AK100</f>
         <v>12.111601290039967</v>
       </c>
@@ -9756,7 +9736,7 @@
       <c r="AY100">
         <v>11.01160293</v>
       </c>
-      <c r="BA100" s="11">
+      <c r="BA100" s="8">
         <f>X100/AY100</f>
         <v>13.915401230327507</v>
       </c>
@@ -9861,7 +9841,7 @@
       <c r="AK101">
         <v>13.29496177</v>
       </c>
-      <c r="AM101" s="11">
+      <c r="AM101" s="8">
         <f>K101/AK101</f>
         <v>13.644761820176337</v>
       </c>
@@ -9898,7 +9878,7 @@
       <c r="AY101">
         <v>66.101127450000007</v>
       </c>
-      <c r="BA101" s="11">
+      <c r="BA101" s="8">
         <f>X101/AY101</f>
         <v>5.3830709586482248</v>
       </c>
@@ -10017,7 +9997,7 @@
       <c r="AK104">
         <v>2.3192826599999998</v>
       </c>
-      <c r="AM104" s="11">
+      <c r="AM104" s="8">
         <f>K104/AK104</f>
         <v>1.8032118948364837</v>
       </c>
@@ -10054,7 +10034,7 @@
       <c r="AY104">
         <v>2.3309191999999999</v>
       </c>
-      <c r="BA104" s="11">
+      <c r="BA104" s="8">
         <f>X104/AY104</f>
         <v>1.6759804629864476</v>
       </c>
@@ -10159,7 +10139,7 @@
       <c r="AK105">
         <v>3.75912282</v>
       </c>
-      <c r="AM105" s="11">
+      <c r="AM105" s="8">
         <f>K105/AK105</f>
         <v>52.61975896813076</v>
       </c>
@@ -10196,7 +10176,7 @@
       <c r="AY105">
         <v>65.975468079999999</v>
       </c>
-      <c r="BA105" s="11">
+      <c r="BA105" s="8">
         <f>X105/AY105</f>
         <v>5.4441983237536737</v>
       </c>
@@ -10315,7 +10295,7 @@
       <c r="AK108">
         <v>3.7323195400000002</v>
       </c>
-      <c r="AM108" s="11">
+      <c r="AM108" s="8">
         <f>K108/AK108</f>
         <v>29.282916346974943</v>
       </c>
@@ -10352,7 +10332,7 @@
       <c r="AY108">
         <v>3.98533874</v>
       </c>
-      <c r="BA108" s="11">
+      <c r="BA108" s="8">
         <f>X108/AY108</f>
         <v>25.389021526436167</v>
       </c>
@@ -10457,7 +10437,7 @@
       <c r="AK109">
         <v>3.7008063</v>
       </c>
-      <c r="AM109" s="11">
+      <c r="AM109" s="8">
         <f>K109/AK109</f>
         <v>52.326704356291216</v>
       </c>
@@ -10494,7 +10474,7 @@
       <c r="AY109">
         <v>65.862993250000002</v>
       </c>
-      <c r="BA109" s="11">
+      <c r="BA109" s="8">
         <f>X109/AY109</f>
         <v>5.4553667319090451</v>
       </c>
@@ -10613,7 +10593,7 @@
       <c r="AK112">
         <v>3.2580644400000001</v>
       </c>
-      <c r="AM112" s="11">
+      <c r="AM112" s="8">
         <f>K112/AK112</f>
         <v>2.2404747402724792</v>
       </c>
@@ -10650,7 +10630,7 @@
       <c r="AY112">
         <v>3.2967851700000002</v>
       </c>
-      <c r="BA112" s="11">
+      <c r="BA112" s="8">
         <f>X112/AY112</f>
         <v>2.2654123471442333</v>
       </c>
@@ -10755,7 +10735,7 @@
       <c r="AK113">
         <v>13.35565901</v>
       </c>
-      <c r="AM113" s="11">
+      <c r="AM113" s="8">
         <f>K113/AK113</f>
         <v>15.372062842146493</v>
       </c>
@@ -10792,7 +10772,7 @@
       <c r="AY113">
         <v>66.190023479999994</v>
       </c>
-      <c r="BA113" s="11">
+      <c r="BA113" s="8">
         <f>X113/AY113</f>
         <v>5.4204200499854549</v>
       </c>
@@ -10911,7 +10891,7 @@
       <c r="AK116">
         <v>12.69277147</v>
       </c>
-      <c r="AM116" s="11">
+      <c r="AM116" s="8">
         <f>K116/AK116</f>
         <v>12.173395754048032</v>
       </c>
@@ -10948,7 +10928,7 @@
       <c r="AY116">
         <v>11.910192390000001</v>
       </c>
-      <c r="BA116" s="11">
+      <c r="BA116" s="8">
         <f>X116/AY116</f>
         <v>12.880919866484206</v>
       </c>
@@ -11053,7 +11033,7 @@
       <c r="AK117">
         <v>13.32009547</v>
       </c>
-      <c r="AM117" s="11">
+      <c r="AM117" s="8">
         <f>K117/AK117</f>
         <v>13.823445293969803</v>
       </c>
@@ -11090,7 +11070,7 @@
       <c r="AY117">
         <v>65.980421890000002</v>
       </c>
-      <c r="BA117" s="11">
+      <c r="BA117" s="8">
         <f>X117/AY117</f>
         <v>5.4153850279358977</v>
       </c>
@@ -11209,7 +11189,7 @@
       <c r="AK120">
         <v>5.4912921800000003</v>
       </c>
-      <c r="AM120" s="11">
+      <c r="AM120" s="8">
         <f>K120/AK120</f>
         <v>1.0210224435735633</v>
       </c>
@@ -11246,7 +11226,7 @@
       <c r="AY120">
         <v>5.4726809200000002</v>
       </c>
-      <c r="BA120" s="11">
+      <c r="BA120" s="8">
         <f>X120/AY120</f>
         <v>1.0237565394183441</v>
       </c>
@@ -11351,7 +11331,7 @@
       <c r="AK121">
         <v>27.748567019999999</v>
       </c>
-      <c r="AM121" s="11">
+      <c r="AM121" s="8">
         <f>K121/AK121</f>
         <v>5.6162025670614248</v>
       </c>
@@ -11388,7 +11368,7 @@
       <c r="AY121">
         <v>66.018213759999995</v>
       </c>
-      <c r="BA121" s="11">
+      <c r="BA121" s="8">
         <f>X121/AY121</f>
         <v>5.4325773852927703</v>
       </c>
@@ -11507,7 +11487,7 @@
       <c r="AK124">
         <v>24.68922439</v>
       </c>
-      <c r="AM124" s="11">
+      <c r="AM124" s="8">
         <f>K124/AK124</f>
         <v>3.9497498706155185</v>
       </c>
@@ -11544,7 +11524,7 @@
       <c r="AY124">
         <v>25.535152969999999</v>
       </c>
-      <c r="BA124" s="11">
+      <c r="BA124" s="8">
         <f>X124/AY124</f>
         <v>3.8735608306794491</v>
       </c>
@@ -11649,7 +11629,7 @@
       <c r="AK125">
         <v>27.144655090000001</v>
       </c>
-      <c r="AM125" s="11">
+      <c r="AM125" s="8">
         <f>K125/AK125</f>
         <v>5.5342425354795699</v>
       </c>
@@ -11686,7 +11666,7 @@
       <c r="AY125">
         <v>65.976099230000003</v>
       </c>
-      <c r="BA125" s="11">
+      <c r="BA125" s="8">
         <f>X125/AY125</f>
         <v>5.4013847529494203</v>
       </c>
@@ -11805,7 +11785,7 @@
       <c r="AK128">
         <v>4.8791888400000003</v>
       </c>
-      <c r="AM128" s="11">
+      <c r="AM128" s="8">
         <f>K128/AK128</f>
         <v>1.9129854892027502</v>
       </c>
@@ -11842,7 +11822,7 @@
       <c r="AY128">
         <v>4.8342177499999996</v>
       </c>
-      <c r="BA128" s="11">
+      <c r="BA128" s="8">
         <f>X128/AY128</f>
         <v>1.9792439304166636</v>
       </c>
@@ -11947,7 +11927,7 @@
       <c r="AK129">
         <v>20.235072049999999</v>
       </c>
-      <c r="AM129" s="11">
+      <c r="AM129" s="8">
         <f>K129/AK129</f>
         <v>8.0710847486208976</v>
       </c>
@@ -11984,7 +11964,7 @@
       <c r="AY129">
         <v>66.278820679999995</v>
       </c>
-      <c r="BA129" s="11">
+      <c r="BA129" s="8">
         <f>X129/AY129</f>
         <v>5.4318707364785297</v>
       </c>
@@ -12103,7 +12083,7 @@
       <c r="AK132">
         <v>18.577346779999999</v>
       </c>
-      <c r="AM132" s="11">
+      <c r="AM132" s="8">
         <f>K132/AK132</f>
         <v>6.071670277018967</v>
       </c>
@@ -12140,7 +12120,7 @@
       <c r="AY132">
         <v>18.455768899999999</v>
       </c>
-      <c r="BA132" s="11">
+      <c r="BA132" s="8">
         <f>X132/AY132</f>
         <v>6.3696702536191818</v>
       </c>
@@ -12245,7 +12225,7 @@
       <c r="AK133">
         <v>19.79816915</v>
       </c>
-      <c r="AM133" s="11">
+      <c r="AM133" s="8">
         <f>K133/AK133</f>
         <v>7.4282726526760676</v>
       </c>
@@ -12282,7 +12262,7 @@
       <c r="AY133">
         <v>66.185822259999995</v>
       </c>
-      <c r="BA133" s="11">
+      <c r="BA133" s="8">
         <f>X133/AY133</f>
         <v>5.3922112773340656</v>
       </c>
@@ -12401,7 +12381,7 @@
       <c r="AK136">
         <v>5.5762620800000002</v>
       </c>
-      <c r="AM136" s="11">
+      <c r="AM136" s="8">
         <f>K136/AK136</f>
         <v>1.0480100372183367</v>
       </c>
@@ -12438,7 +12418,7 @@
       <c r="AY136">
         <v>5.4681502100000001</v>
       </c>
-      <c r="BA136" s="11">
+      <c r="BA136" s="8">
         <f>X136/AY136</f>
         <v>1.0327779894693125</v>
       </c>
@@ -12543,7 +12523,7 @@
       <c r="AK137">
         <v>27.665271570000002</v>
       </c>
-      <c r="AM137" s="11">
+      <c r="AM137" s="8">
         <f>K137/AK137</f>
         <v>5.6531679349063406</v>
       </c>
@@ -12580,7 +12560,7 @@
       <c r="AY137">
         <v>66.110330610000005</v>
       </c>
-      <c r="BA137" s="11">
+      <c r="BA137" s="8">
         <f>X137/AY137</f>
         <v>5.4562945730517498</v>
       </c>
@@ -12699,7 +12679,7 @@
       <c r="AK140">
         <v>24.866776250000001</v>
       </c>
-      <c r="AM140" s="11">
+      <c r="AM140" s="8">
         <f>K140/AK140</f>
         <v>4.0119617696724967</v>
       </c>
@@ -12736,7 +12716,7 @@
       <c r="AY140">
         <v>25.55335797</v>
       </c>
-      <c r="BA140" s="11">
+      <c r="BA140" s="8">
         <f>X140/AY140</f>
         <v>3.9478446836003056</v>
       </c>
@@ -12841,7 +12821,7 @@
       <c r="AK141">
         <v>27.2027006</v>
       </c>
-      <c r="AM141" s="11">
+      <c r="AM141" s="8">
         <f>K141/AK141</f>
         <v>5.518807166520812</v>
       </c>
@@ -12878,7 +12858,7 @@
       <c r="AY141">
         <v>66.059024930000007</v>
       </c>
-      <c r="BA141" s="11">
+      <c r="BA141" s="8">
         <f>X141/AY141</f>
         <v>5.4275003807568307</v>
       </c>
@@ -12997,7 +12977,7 @@
       <c r="AK144">
         <v>4.7601072499999999</v>
       </c>
-      <c r="AM144" s="11">
+      <c r="AM144" s="8">
         <f>K144/AK144</f>
         <v>1.9781217597565686</v>
       </c>
@@ -13034,7 +13014,7 @@
       <c r="AY144">
         <v>4.7017625000000001</v>
       </c>
-      <c r="BA144" s="11">
+      <c r="BA144" s="8">
         <f>X144/AY144</f>
         <v>2.0086584764755768</v>
       </c>
@@ -13139,7 +13119,7 @@
       <c r="AK145">
         <v>20.15633089</v>
       </c>
-      <c r="AM145" s="11">
+      <c r="AM145" s="8">
         <f>K145/AK145</f>
         <v>8.118064566561598</v>
       </c>
@@ -13176,7 +13156,7 @@
       <c r="AY145">
         <v>66.361536319999999</v>
       </c>
-      <c r="BA145" s="11">
+      <c r="BA145" s="8">
         <f>X145/AY145</f>
         <v>5.4754024261564895</v>
       </c>
@@ -13295,7 +13275,7 @@
       <c r="AK148">
         <v>18.128191690000001</v>
       </c>
-      <c r="AM148" s="11">
+      <c r="AM148" s="8">
         <f>K148/AK148</f>
         <v>7.065347424070624</v>
       </c>
@@ -13332,7 +13312,7 @@
       <c r="AY148">
         <v>18.176662619999998</v>
       </c>
-      <c r="BA148" s="11">
+      <c r="BA148" s="8">
         <f>X148/AY148</f>
         <v>7.333555498979714</v>
       </c>
@@ -13437,7 +13417,7 @@
       <c r="AK149">
         <v>19.781847760000002</v>
       </c>
-      <c r="AM149" s="11">
+      <c r="AM149" s="8">
         <f>K149/AK149</f>
         <v>7.4185653322407319</v>
       </c>
@@ -13474,7 +13454,7 @@
       <c r="AY149">
         <v>66.142824320000003</v>
       </c>
-      <c r="BA149" s="11">
+      <c r="BA149" s="8">
         <f>X149/AY149</f>
         <v>5.4535098214868611</v>
       </c>
@@ -13593,7 +13573,7 @@
       <c r="AK152">
         <v>2.8364063000000002</v>
       </c>
-      <c r="AM152" s="11">
+      <c r="AM152" s="8">
         <f>K152/AK152</f>
         <v>0.9985987938328863</v>
       </c>
@@ -13630,7 +13610,7 @@
       <c r="AY152">
         <v>2.7735373499999998</v>
       </c>
-      <c r="BA152" s="11">
+      <c r="BA152" s="8">
         <f>X152/AY152</f>
         <v>1.1005523037214553</v>
       </c>
@@ -13735,7 +13715,7 @@
       <c r="AK153">
         <v>5.6348140400000002</v>
       </c>
-      <c r="AM153" s="11">
+      <c r="AM153" s="8">
         <f>K153/AK153</f>
         <v>108.51546569050574</v>
       </c>
@@ -13772,7 +13752,7 @@
       <c r="AY153">
         <v>10.274385690000001</v>
       </c>
-      <c r="BA153" s="11">
+      <c r="BA153" s="8">
         <f>X153/AY153</f>
         <v>5.5449799792361114</v>
       </c>
@@ -13891,7 +13871,7 @@
       <c r="AK156">
         <v>4.8515357300000002</v>
       </c>
-      <c r="AM156" s="11">
+      <c r="AM156" s="8">
         <f>K156/AK156</f>
         <v>5.3954803874030208</v>
       </c>
@@ -13928,7 +13908,7 @@
       <c r="AY156">
         <v>5.0534171499999996</v>
       </c>
-      <c r="BA156" s="11">
+      <c r="BA156" s="8">
         <f>X156/AY156</f>
         <v>5.4210413818696921</v>
       </c>
@@ -14033,7 +14013,7 @@
       <c r="AK157">
         <v>5.55246336</v>
       </c>
-      <c r="AM157" s="11">
+      <c r="AM157" s="8">
         <f>K157/AK157</f>
         <v>78.967367330812976</v>
       </c>
@@ -14070,7 +14050,7 @@
       <c r="AY157">
         <v>9.7260405799999994</v>
       </c>
-      <c r="BA157" s="11">
+      <c r="BA157" s="8">
         <f>X157/AY157</f>
         <v>4.0865931139267371</v>
       </c>
@@ -14189,7 +14169,7 @@
       <c r="AK160">
         <v>3.1857431599999999</v>
       </c>
-      <c r="AM160" s="11">
+      <c r="AM160" s="8">
         <f>K160/AK160</f>
         <v>1.7273811866239714</v>
       </c>
@@ -14226,7 +14206,7 @@
       <c r="AY160">
         <v>2.7983142999999999</v>
       </c>
-      <c r="BA160" s="11">
+      <c r="BA160" s="8">
         <f>X160/AY160</f>
         <v>2.020150738607168</v>
       </c>
@@ -14331,7 +14311,7 @@
       <c r="AK161">
         <v>26.806040209999999</v>
       </c>
-      <c r="AM161" s="11">
+      <c r="AM161" s="8">
         <f>K161/AK161</f>
         <v>15.867524018386154</v>
       </c>
@@ -14368,7 +14348,7 @@
       <c r="AY161">
         <v>30.506092720000002</v>
       </c>
-      <c r="BA161" s="11">
+      <c r="BA161" s="8">
         <f>X161/AY161</f>
         <v>1.8323145872219062</v>
       </c>
@@ -14487,7 +14467,7 @@
       <c r="AK164">
         <v>12.87745428</v>
       </c>
-      <c r="AM164" s="11">
+      <c r="AM164" s="8">
         <f>K164/AK164</f>
         <v>1.9504519778423159</v>
       </c>
@@ -14524,7 +14504,7 @@
       <c r="AY164">
         <v>4.2077058200000002</v>
       </c>
-      <c r="BA164" s="11">
+      <c r="BA164" s="8">
         <f>X164/AY164</f>
         <v>5.9028605402836831</v>
       </c>
@@ -14629,7 +14609,7 @@
       <c r="AK165">
         <v>25.730250229999999</v>
       </c>
-      <c r="AM165" s="11">
+      <c r="AM165" s="8">
         <f>K165/AK165</f>
         <v>12.311621368946165</v>
       </c>
@@ -14666,7 +14646,7 @@
       <c r="AY165">
         <v>25.44896103</v>
       </c>
-      <c r="BA165" s="11">
+      <c r="BA165" s="8">
         <f>X165/AY165</f>
         <v>1.4750125195975436</v>
       </c>
@@ -14785,7 +14765,7 @@
       <c r="AK168">
         <v>2.8732180999999999</v>
       </c>
-      <c r="AM168" s="11">
+      <c r="AM168" s="8">
         <f>K168/AK168</f>
         <v>1.0560510669203986</v>
       </c>
@@ -14822,7 +14802,7 @@
       <c r="AY168">
         <v>2.7947668499999998</v>
       </c>
-      <c r="BA168" s="11">
+      <c r="BA168" s="8">
         <f>X168/AY168</f>
         <v>1.1033212376910797</v>
       </c>
@@ -14927,7 +14907,7 @@
       <c r="AK169">
         <v>5.5960717999999998</v>
       </c>
-      <c r="AM169" s="11">
+      <c r="AM169" s="8">
         <f>K169/AK169</f>
         <v>103.38616207711988</v>
       </c>
@@ -14964,7 +14944,7 @@
       <c r="AY169">
         <v>10.31898724</v>
       </c>
-      <c r="BA169" s="11">
+      <c r="BA169" s="8">
         <f>X169/AY169</f>
         <v>5.333962068161255</v>
       </c>
@@ -15083,7 +15063,7 @@
       <c r="AK172">
         <v>4.8676936499999996</v>
       </c>
-      <c r="AM172" s="11">
+      <c r="AM172" s="8">
         <f>K172/AK172</f>
         <v>5.3482271198393931</v>
       </c>
@@ -15120,7 +15100,7 @@
       <c r="AY172">
         <v>4.9371135199999996</v>
       </c>
-      <c r="BA172" s="11">
+      <c r="BA172" s="8">
         <f>X172/AY172</f>
         <v>5.5539484070846328</v>
       </c>
@@ -15225,7 +15205,7 @@
       <c r="AK173">
         <v>5.51351236</v>
       </c>
-      <c r="AM173" s="11">
+      <c r="AM173" s="8">
         <f>K173/AK173</f>
         <v>84.102341665921287</v>
       </c>
@@ -15262,7 +15242,7 @@
       <c r="AY173">
         <v>9.6914977199999992</v>
       </c>
-      <c r="BA173" s="11">
+      <c r="BA173" s="8">
         <f>X173/AY173</f>
         <v>4.0817731874779835</v>
       </c>
@@ -15381,7 +15361,7 @@
       <c r="AK176">
         <v>3.07502319</v>
       </c>
-      <c r="AM176" s="11">
+      <c r="AM176" s="8">
         <f>K176/AK176</f>
         <v>1.8482526858602324</v>
       </c>
@@ -15418,7 +15398,7 @@
       <c r="AY176">
         <v>3.1201773799999999</v>
       </c>
-      <c r="BA176" s="11">
+      <c r="BA176" s="8">
         <f>X176/AY176</f>
         <v>1.8368168478934361</v>
       </c>
@@ -15523,7 +15503,7 @@
       <c r="AK177">
         <v>26.834354909999998</v>
       </c>
-      <c r="AM177" s="11">
+      <c r="AM177" s="8">
         <f>K177/AK177</f>
         <v>15.746937080739388</v>
       </c>
@@ -15560,7 +15540,7 @@
       <c r="AY177">
         <v>30.83725205</v>
       </c>
-      <c r="BA177" s="11">
+      <c r="BA177" s="8">
         <f>X177/AY177</f>
         <v>1.8181711197577346</v>
       </c>
@@ -15679,7 +15659,7 @@
       <c r="AK180">
         <v>14.398661499999999</v>
       </c>
-      <c r="AM180" s="11">
+      <c r="AM180" s="8">
         <f>K180/AK180</f>
         <v>2.2586613415420591</v>
       </c>
@@ -15716,7 +15696,7 @@
       <c r="AY180">
         <v>14.67170591</v>
       </c>
-      <c r="BA180" s="11">
+      <c r="BA180" s="8">
         <f>X180/AY180</f>
         <v>1.9990907676256715</v>
       </c>
@@ -15821,7 +15801,7 @@
       <c r="AK181">
         <v>25.851305459999999</v>
       </c>
-      <c r="AM181" s="11">
+      <c r="AM181" s="8">
         <f>K181/AK181</f>
         <v>11.890890134180481</v>
       </c>
@@ -15858,7 +15838,7 @@
       <c r="AY181">
         <v>23.596449</v>
       </c>
-      <c r="BA181" s="11">
+      <c r="BA181" s="8">
         <f>X181/AY181</f>
         <v>1.5220813038436418</v>
       </c>
@@ -15977,7 +15957,7 @@
       <c r="AK184">
         <v>2.34018579</v>
       </c>
-      <c r="AM184" s="11">
+      <c r="AM184" s="8">
         <f>K184/AK184</f>
         <v>1.3006497189268038</v>
       </c>
@@ -16014,7 +15994,7 @@
       <c r="AY184">
         <v>2.3709031399999998</v>
       </c>
-      <c r="BA184" s="11">
+      <c r="BA184" s="8">
         <f>X184/AY184</f>
         <v>1.2861328658074156</v>
       </c>
@@ -16119,7 +16099,7 @@
       <c r="AK185">
         <v>5.6740824099999996</v>
       </c>
-      <c r="AM185" s="11">
+      <c r="AM185" s="8">
         <f>K185/AK185</f>
         <v>153.65993049262039</v>
       </c>
@@ -16156,7 +16136,7 @@
       <c r="AY185">
         <v>10.68362623</v>
       </c>
-      <c r="BA185" s="11">
+      <c r="BA185" s="8">
         <f>X185/AY185</f>
         <v>5.7262852923674403</v>
       </c>
@@ -16275,7 +16255,7 @@
       <c r="AK188">
         <v>4.9957086899999998</v>
       </c>
-      <c r="AM188" s="11">
+      <c r="AM188" s="8">
         <f>K188/AK188</f>
         <v>5.801929799873899</v>
       </c>
@@ -16312,7 +16292,7 @@
       <c r="AY188">
         <v>5.1694520500000003</v>
       </c>
-      <c r="BA188" s="11">
+      <c r="BA188" s="8">
         <f>X188/AY188</f>
         <v>5.7105943733436888</v>
       </c>
@@ -16417,7 +16397,7 @@
       <c r="AK189">
         <v>5.60675627</v>
       </c>
-      <c r="AM189" s="11">
+      <c r="AM189" s="8">
         <f>K189/AK189</f>
         <v>105.90609685446519</v>
       </c>
@@ -16454,7 +16434,7 @@
       <c r="AY189">
         <v>9.8733280600000004</v>
       </c>
-      <c r="BA189" s="11">
+      <c r="BA189" s="8">
         <f>X189/AY189</f>
         <v>4.0949674268191991</v>
       </c>
@@ -16573,7 +16553,7 @@
       <c r="AK192">
         <v>2.6342534099999999</v>
       </c>
-      <c r="AM192" s="11">
+      <c r="AM192" s="8">
         <f>K192/AK192</f>
         <v>1.7562397119569451</v>
       </c>
@@ -16610,7 +16590,7 @@
       <c r="AY192">
         <v>2.6902215300000001</v>
       </c>
-      <c r="BA192" s="11">
+      <c r="BA192" s="8">
         <f>X192/AY192</f>
         <v>1.7502338961654209</v>
       </c>
@@ -16715,7 +16695,7 @@
       <c r="AK193">
         <v>29.695561699999999</v>
       </c>
-      <c r="AM193" s="11">
+      <c r="AM193" s="8">
         <f>K193/AK193</f>
         <v>26.637093153216902</v>
       </c>
@@ -16752,7 +16732,7 @@
       <c r="AY193">
         <v>34.318958960000003</v>
       </c>
-      <c r="BA193" s="11">
+      <c r="BA193" s="8">
         <f>X193/AY193</f>
         <v>1.7474248819696712</v>
       </c>
@@ -16871,7 +16851,7 @@
       <c r="AK196">
         <v>13.28520546</v>
       </c>
-      <c r="AM196" s="11">
+      <c r="AM196" s="8">
         <f>K196/AK196</f>
         <v>1.9628483216547858</v>
       </c>
@@ -16908,7 +16888,7 @@
       <c r="AY196">
         <v>11.320810249999999</v>
       </c>
-      <c r="BA196" s="11">
+      <c r="BA196" s="8">
         <f>X196/AY196</f>
         <v>2.3036654545110853</v>
       </c>
@@ -17013,7 +16993,7 @@
       <c r="AK197">
         <v>28.45027915</v>
       </c>
-      <c r="AM197" s="11">
+      <c r="AM197" s="8">
         <f>K197/AK197</f>
         <v>17.399756844916581</v>
       </c>
@@ -17050,7 +17030,7 @@
       <c r="AY197">
         <v>28.042410889999999</v>
       </c>
-      <c r="BA197" s="11">
+      <c r="BA197" s="8">
         <f>X197/AY197</f>
         <v>1.3370557141850652</v>
       </c>
@@ -17169,7 +17149,7 @@
       <c r="AK200">
         <v>2.3477137799999999</v>
       </c>
-      <c r="AM200" s="11">
+      <c r="AM200" s="8">
         <f>K200/AK200</f>
         <v>1.2739876366019371</v>
       </c>
@@ -17206,7 +17186,7 @@
       <c r="AY200">
         <v>2.35428229</v>
       </c>
-      <c r="BA200" s="11">
+      <c r="BA200" s="8">
         <f>X200/AY200</f>
         <v>1.2886974441794743</v>
       </c>
@@ -17311,7 +17291,7 @@
       <c r="AK201">
         <v>5.6626635500000004</v>
       </c>
-      <c r="AM201" s="11">
+      <c r="AM201" s="8">
         <f>K201/AK201</f>
         <v>153.40149505085816</v>
       </c>
@@ -17348,7 +17328,7 @@
       <c r="AY201">
         <v>10.66096797</v>
       </c>
-      <c r="BA201" s="11">
+      <c r="BA201" s="8">
         <f>X201/AY201</f>
         <v>5.7305756008194821</v>
       </c>
@@ -17467,7 +17447,7 @@
       <c r="AK204">
         <v>4.9557304599999998</v>
       </c>
-      <c r="AM204" s="11">
+      <c r="AM204" s="8">
         <f>K204/AK204</f>
         <v>6.0709974791486143</v>
       </c>
@@ -17504,7 +17484,7 @@
       <c r="AY204">
         <v>5.1806572900000001</v>
       </c>
-      <c r="BA204" s="11">
+      <c r="BA204" s="8">
         <f>X204/AY204</f>
         <v>5.6089458042494833</v>
       </c>
@@ -17609,7 +17589,7 @@
       <c r="AK205">
         <v>5.60160225</v>
       </c>
-      <c r="AM205" s="11">
+      <c r="AM205" s="8">
         <f>K205/AK205</f>
         <v>105.90939758887737</v>
       </c>
@@ -17646,7 +17626,7 @@
       <c r="AY205">
         <v>9.8669777500000002</v>
       </c>
-      <c r="BA205" s="11">
+      <c r="BA205" s="8">
         <f>X205/AY205</f>
         <v>4.085859189253771</v>
       </c>
@@ -17765,7 +17745,7 @@
       <c r="AK208">
         <v>2.57171021</v>
       </c>
-      <c r="AM208" s="11">
+      <c r="AM208" s="8">
         <f>K208/AK208</f>
         <v>1.7766961581569487</v>
       </c>
@@ -17802,7 +17782,7 @@
       <c r="AY208">
         <v>2.6375933499999999</v>
       </c>
-      <c r="BA208" s="11">
+      <c r="BA208" s="8">
         <f>X208/AY208</f>
         <v>1.7044135556377558</v>
       </c>
@@ -17907,7 +17887,7 @@
       <c r="AK209">
         <v>29.71521826</v>
       </c>
-      <c r="AM209" s="11">
+      <c r="AM209" s="8">
         <f>K209/AK209</f>
         <v>27.033436747841005</v>
       </c>
@@ -17944,7 +17924,7 @@
       <c r="AY209">
         <v>34.82631542</v>
       </c>
-      <c r="BA209" s="11">
+      <c r="BA209" s="8">
         <f>X209/AY209</f>
         <v>1.7221876318720828</v>
       </c>
@@ -18063,7 +18043,7 @@
       <c r="AK212">
         <v>14.78498201</v>
       </c>
-      <c r="AM212" s="11">
+      <c r="AM212" s="8">
         <f>K212/AK212</f>
         <v>2.2507137862929332</v>
       </c>
@@ -18100,7 +18080,7 @@
       <c r="AY212">
         <v>14.97997178</v>
       </c>
-      <c r="BA212" s="11">
+      <c r="BA212" s="8">
         <f>X212/AY212</f>
         <v>2.1177392438318732</v>
       </c>
@@ -18205,7 +18185,7 @@
       <c r="AK213">
         <v>28.508706159999999</v>
       </c>
-      <c r="AM213" s="11">
+      <c r="AM213" s="8">
         <f>K213/AK213</f>
         <v>16.823680633495297</v>
       </c>
@@ -18242,7 +18222,7 @@
       <c r="AY213">
         <v>25.839473460000001</v>
       </c>
-      <c r="BA213" s="11">
+      <c r="BA213" s="8">
         <f>X213/AY213</f>
         <v>1.4402237683987233</v>
       </c>
@@ -18361,7 +18341,7 @@
       <c r="AK216">
         <v>2.5107390600000001</v>
       </c>
-      <c r="AM216" s="11">
+      <c r="AM216" s="8">
         <f>K216/AK216</f>
         <v>1.3202304424259841</v>
       </c>
@@ -18398,7 +18378,7 @@
       <c r="AY216">
         <v>2.5316673600000001</v>
       </c>
-      <c r="BA216" s="11">
+      <c r="BA216" s="8">
         <f>X216/AY216</f>
         <v>1.293991506056309</v>
       </c>
@@ -18503,7 +18483,7 @@
       <c r="AK217">
         <v>5.6506155800000002</v>
       </c>
-      <c r="AM217" s="11">
+      <c r="AM217" s="8">
         <f>K217/AK217</f>
         <v>164.08207351631589</v>
       </c>
@@ -18540,7 +18520,7 @@
       <c r="AY217">
         <v>12.889155840000001</v>
       </c>
-      <c r="BA217" s="11">
+      <c r="BA217" s="8">
         <f>X217/AY217</f>
         <v>112.10950762544275</v>
       </c>
@@ -18659,7 +18639,7 @@
       <c r="AK220">
         <v>5.50358035</v>
       </c>
-      <c r="AM220" s="11">
+      <c r="AM220" s="8">
         <f>K220/AK220</f>
         <v>24.659007958337522</v>
       </c>
@@ -18696,7 +18676,7 @@
       <c r="AY220">
         <v>5.71498784</v>
       </c>
-      <c r="BA220" s="11">
+      <c r="BA220" s="8">
         <f>X220/AY220</f>
         <v>22.91014193479019</v>
       </c>
@@ -18801,7 +18781,7 @@
       <c r="AK221">
         <v>5.6039451900000001</v>
       </c>
-      <c r="AM221" s="11">
+      <c r="AM221" s="8">
         <f>K221/AK221</f>
         <v>105.14316127884898</v>
       </c>
@@ -18838,7 +18818,7 @@
       <c r="AY221">
         <v>12.539332910000001</v>
       </c>
-      <c r="BA221" s="11">
+      <c r="BA221" s="8">
         <f>X221/AY221</f>
         <v>56.993046405209441</v>
       </c>
@@ -18957,7 +18937,7 @@
       <c r="AK224">
         <v>2.6274013799999998</v>
       </c>
-      <c r="AM224" s="11">
+      <c r="AM224" s="8">
         <f>K224/AK224</f>
         <v>1.763844007724469</v>
       </c>
@@ -18994,7 +18974,7 @@
       <c r="AY224">
         <v>2.7096423199999999</v>
       </c>
-      <c r="BA224" s="11">
+      <c r="BA224" s="8">
         <f>X224/AY224</f>
         <v>1.7418048851554695</v>
       </c>
@@ -19099,7 +19079,7 @@
       <c r="AK225">
         <v>29.708732319999999</v>
       </c>
-      <c r="AM225" s="11">
+      <c r="AM225" s="8">
         <f>K225/AK225</f>
         <v>27.022146670645959</v>
       </c>
@@ -19136,7 +19116,7 @@
       <c r="AY225">
         <v>34.51088618</v>
       </c>
-      <c r="BA225" s="11">
+      <c r="BA225" s="8">
         <f>X225/AY225</f>
         <v>1.7404189566945512</v>
       </c>
@@ -19255,7 +19235,7 @@
       <c r="AK228">
         <v>13.1781822</v>
       </c>
-      <c r="AM228" s="11">
+      <c r="AM228" s="8">
         <f>K228/AK228</f>
         <v>1.9501783569208808</v>
       </c>
@@ -19292,7 +19272,7 @@
       <c r="AY228">
         <v>12.28860527</v>
       </c>
-      <c r="BA228" s="11">
+      <c r="BA228" s="8">
         <f>X228/AY228</f>
         <v>2.1008767400989194</v>
       </c>
@@ -19397,7 +19377,7 @@
       <c r="AK229">
         <v>28.4424332</v>
       </c>
-      <c r="AM229" s="11">
+      <c r="AM229" s="8">
         <f>K229/AK229</f>
         <v>17.274159511430266</v>
       </c>
@@ -19434,7 +19414,7 @@
       <c r="AY229">
         <v>28.121860460000001</v>
       </c>
-      <c r="BA229" s="11">
+      <c r="BA229" s="8">
         <f>X229/AY229</f>
         <v>1.3300314871841874</v>
       </c>
@@ -19553,7 +19533,7 @@
       <c r="AK232">
         <v>2.4939136</v>
       </c>
-      <c r="AM232" s="11">
+      <c r="AM232" s="8">
         <f>K232/AK232</f>
         <v>1.3079275881891017</v>
       </c>
@@ -19590,7 +19570,7 @@
       <c r="AY232">
         <v>2.4237658999999998</v>
       </c>
-      <c r="BA232" s="11">
+      <c r="BA232" s="8">
         <f>X232/AY232</f>
         <v>1.338440032513041</v>
       </c>
@@ -19695,7 +19675,7 @@
       <c r="AK233">
         <v>5.64399008</v>
       </c>
-      <c r="AM233" s="11">
+      <c r="AM233" s="8">
         <f>K233/AK233</f>
         <v>162.81509251873101</v>
       </c>
@@ -19732,7 +19712,7 @@
       <c r="AY233">
         <v>12.76904294</v>
       </c>
-      <c r="BA233" s="11">
+      <c r="BA233" s="8">
         <f>X233/AY233</f>
         <v>111.84768230719099</v>
       </c>
@@ -19851,7 +19831,7 @@
       <c r="AK236">
         <v>5.4934882900000002</v>
       </c>
-      <c r="AM236" s="11">
+      <c r="AM236" s="8">
         <f>K236/AK236</f>
         <v>25.278596341560597</v>
       </c>
@@ -19888,7 +19868,7 @@
       <c r="AY236">
         <v>5.6779436299999997</v>
       </c>
-      <c r="BA236" s="11">
+      <c r="BA236" s="8">
         <f>X236/AY236</f>
         <v>23.091358448375441</v>
       </c>
@@ -19993,7 +19973,7 @@
       <c r="AK237">
         <v>5.5959557799999997</v>
       </c>
-      <c r="AM237" s="11">
+      <c r="AM237" s="8">
         <f>K237/AK237</f>
         <v>103.29346470818611</v>
       </c>
@@ -20030,7 +20010,7 @@
       <c r="AY237">
         <v>12.48001637</v>
       </c>
-      <c r="BA237" s="11">
+      <c r="BA237" s="8">
         <f>X237/AY237</f>
         <v>57.549523012364446</v>
       </c>
@@ -20149,7 +20129,7 @@
       <c r="AK240">
         <v>2.4427093100000001</v>
       </c>
-      <c r="AM240" s="11">
+      <c r="AM240" s="8">
         <f>K240/AK240</f>
         <v>1.8472727317684803</v>
       </c>
@@ -20186,7 +20166,7 @@
       <c r="AY240">
         <v>2.6357788499999999</v>
       </c>
-      <c r="BA240" s="11">
+      <c r="BA240" s="8">
         <f>X240/AY240</f>
         <v>1.6777649611992298</v>
       </c>
@@ -20291,7 +20271,7 @@
       <c r="AK241">
         <v>29.706208270000001</v>
       </c>
-      <c r="AM241" s="11">
+      <c r="AM241" s="8">
         <f>K241/AK241</f>
         <v>26.772461498668406</v>
       </c>
@@ -20328,7 +20308,7 @@
       <c r="AY241">
         <v>34.338730150000004</v>
       </c>
-      <c r="BA241" s="11">
+      <c r="BA241" s="8">
         <f>X241/AY241</f>
         <v>1.7645390116442612</v>
       </c>
@@ -20447,7 +20427,7 @@
       <c r="AK244">
         <v>15.37872415</v>
       </c>
-      <c r="AM244" s="11">
+      <c r="AM244" s="8">
         <f>K244/AK244</f>
         <v>2.1549691129611683</v>
       </c>
@@ -20484,7 +20464,7 @@
       <c r="AY244">
         <v>15.21585979</v>
       </c>
-      <c r="BA244" s="11">
+      <c r="BA244" s="8">
         <f>X244/AY244</f>
         <v>2.1121120195337975</v>
       </c>
@@ -20589,7 +20569,7 @@
       <c r="AK245">
         <v>28.528403659999999</v>
       </c>
-      <c r="AM245" s="11">
+      <c r="AM245" s="8">
         <f>K245/AK245</f>
         <v>16.364703138107519</v>
       </c>
@@ -20626,7 +20606,7 @@
       <c r="AY245">
         <v>25.852765089999998</v>
       </c>
-      <c r="BA245" s="11">
+      <c r="BA245" s="8">
         <f>X245/AY245</f>
         <v>1.4336649716566161</v>
       </c>
@@ -20720,7 +20700,7 @@
       </c>
     </row>
     <row r="249" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="AM249" s="11"/>
+      <c r="AM249" s="8"/>
     </row>
     <row r="250" spans="1:53" ht="43.2" x14ac:dyDescent="0.3">
       <c r="H250" s="5" t="s">
@@ -20783,52 +20763,52 @@
       </c>
     </row>
     <row r="252" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="AM252" s="11"/>
+      <c r="AM252" s="8"/>
     </row>
     <row r="253" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="AM253" s="11"/>
+      <c r="AM253" s="8"/>
     </row>
     <row r="256" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="AM256" s="11"/>
+      <c r="AM256" s="8"/>
     </row>
     <row r="257" spans="39:39" x14ac:dyDescent="0.3">
-      <c r="AM257" s="11"/>
+      <c r="AM257" s="8"/>
     </row>
     <row r="260" spans="39:39" x14ac:dyDescent="0.3">
-      <c r="AM260" s="11"/>
+      <c r="AM260" s="8"/>
     </row>
     <row r="261" spans="39:39" x14ac:dyDescent="0.3">
-      <c r="AM261" s="11"/>
+      <c r="AM261" s="8"/>
     </row>
     <row r="264" spans="39:39" x14ac:dyDescent="0.3">
-      <c r="AM264" s="11"/>
+      <c r="AM264" s="8"/>
     </row>
     <row r="265" spans="39:39" x14ac:dyDescent="0.3">
-      <c r="AM265" s="11"/>
+      <c r="AM265" s="8"/>
     </row>
     <row r="268" spans="39:39" x14ac:dyDescent="0.3">
-      <c r="AM268" s="11"/>
+      <c r="AM268" s="8"/>
     </row>
     <row r="269" spans="39:39" x14ac:dyDescent="0.3">
-      <c r="AM269" s="11"/>
+      <c r="AM269" s="8"/>
     </row>
     <row r="272" spans="39:39" x14ac:dyDescent="0.3">
-      <c r="AM272" s="11"/>
+      <c r="AM272" s="8"/>
     </row>
     <row r="273" spans="39:39" x14ac:dyDescent="0.3">
-      <c r="AM273" s="11"/>
+      <c r="AM273" s="8"/>
     </row>
     <row r="276" spans="39:39" x14ac:dyDescent="0.3">
-      <c r="AM276" s="11"/>
+      <c r="AM276" s="8"/>
     </row>
     <row r="277" spans="39:39" x14ac:dyDescent="0.3">
-      <c r="AM277" s="11"/>
+      <c r="AM277" s="8"/>
     </row>
     <row r="280" spans="39:39" x14ac:dyDescent="0.3">
-      <c r="AM280" s="11"/>
+      <c r="AM280" s="8"/>
     </row>
     <row r="281" spans="39:39" x14ac:dyDescent="0.3">
-      <c r="AM281" s="11"/>
+      <c r="AM281" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -20849,6 +20829,35 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="K1:K246">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K247:K248">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N3:N245">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>A3&lt;&gt;N3</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="X1">
     <cfRule type="colorScale" priority="37">
       <colorScale>
@@ -20861,8 +20870,66 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="X1:X246 X249 X252:X1048576">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X247:X248">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA3:AA245">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>A3&lt;&gt;AA3</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="AK1:AL1">
     <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK1:AL249 AK251:AL1048576 AL250">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AO3:AO245">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>A3&lt;&gt;AO3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AY247:AY248">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -20885,80 +20952,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K1:K246">
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X1:X246 X249 X252:X1048576">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK1:AL249 AK251:AL1048576 AL250">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="AY1:AZ246 AY249:AZ249 AY251:AZ1048576 AZ250">
     <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K247:K248">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X247:X248">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AY247:AY248">
-    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -20981,21 +20976,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3:N245">
-    <cfRule type="expression" dxfId="5" priority="3">
-      <formula>A3&lt;&gt;N3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA3:AA245">
-    <cfRule type="expression" dxfId="4" priority="2">
-      <formula>A3&lt;&gt;AA3</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AO3:AO245">
-    <cfRule type="expression" dxfId="3" priority="1">
-      <formula>A3&lt;&gt;AO3</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>